<commit_message>
Main loop and other stuff
</commit_message>
<xml_diff>
--- a/SignalsSignalsSignals_004.xlsx
+++ b/SignalsSignalsSignals_004.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="194">
   <si>
     <t xml:space="preserve">Light Signals:</t>
   </si>
@@ -546,6 +546,12 @@
   </si>
   <si>
     <t xml:space="preserve">S4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V14</t>
   </si>
   <si>
     <t xml:space="preserve">to city station</t>
@@ -1098,7 +1104,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1399,6 +1405,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1646,9 +1660,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>132480</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>113040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1662,7 +1676,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3431520" y="2295360"/>
-          <a:ext cx="1579320" cy="2580480"/>
+          <a:ext cx="1578960" cy="2580120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1683,9 +1697,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>142200</xdr:colOff>
+      <xdr:colOff>141840</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>189720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1699,7 +1713,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3421800" y="6153120"/>
-          <a:ext cx="1598400" cy="3561840"/>
+          <a:ext cx="1598040" cy="3561480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1720,9 +1734,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>161280</xdr:colOff>
+      <xdr:colOff>160920</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1736,7 +1750,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3393360" y="11049120"/>
-          <a:ext cx="3130560" cy="3418920"/>
+          <a:ext cx="3130200" cy="3418560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1757,9 +1771,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>85680</xdr:colOff>
+      <xdr:colOff>85320</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1773,7 +1787,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3393360" y="17525880"/>
-          <a:ext cx="2418840" cy="4800240"/>
+          <a:ext cx="2418480" cy="4799880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1794,9 +1808,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
+      <xdr:colOff>46440</xdr:colOff>
       <xdr:row>116</xdr:row>
-      <xdr:rowOff>175680</xdr:rowOff>
+      <xdr:rowOff>175320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1810,7 +1824,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7211160" y="17907120"/>
-          <a:ext cx="4712760" cy="4366440"/>
+          <a:ext cx="4712400" cy="4366080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1831,9 +1845,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>137880</xdr:colOff>
+      <xdr:colOff>137520</xdr:colOff>
       <xdr:row>150</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:rowOff>75240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1847,7 +1861,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3362400" y="24717600"/>
-          <a:ext cx="5471280" cy="3933000"/>
+          <a:ext cx="5470920" cy="3932640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1868,9 +1882,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>149</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1884,7 +1898,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8965080" y="24765120"/>
-          <a:ext cx="4693680" cy="3776040"/>
+          <a:ext cx="4693320" cy="3775680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1953,9 +1967,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>113</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1965,7 +1979,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18825840" y="3284640"/>
-          <a:ext cx="5206320" cy="934200"/>
+          <a:ext cx="5205960" cy="933840"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2171,9 +2185,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>161</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>27360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2183,7 +2197,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="29006280" y="3284640"/>
-          <a:ext cx="5205960" cy="934200"/>
+          <a:ext cx="5205600" cy="933840"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2244,15 +2258,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>-720</xdr:colOff>
       <xdr:row>149</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>157</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2261,8 +2275,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9119880" y="28422720"/>
-          <a:ext cx="1069200" cy="1675440"/>
+          <a:off x="9119160" y="28422720"/>
+          <a:ext cx="1068840" cy="1675080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2312,9 +2326,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
-      <xdr:colOff>189720</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2328,7 +2342,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9265320" y="2752560"/>
-          <a:ext cx="2589480" cy="2361600"/>
+          <a:ext cx="2589120" cy="2361240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2349,9 +2363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
-      <xdr:colOff>37440</xdr:colOff>
+      <xdr:colOff>37080</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2360,8 +2374,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7306560" y="3751920"/>
-          <a:ext cx="3547440" cy="980280"/>
+          <a:off x="7306560" y="3752280"/>
+          <a:ext cx="3547080" cy="979920"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2406,15 +2420,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>-720</xdr:colOff>
       <xdr:row>175</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>183</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2423,8 +2437,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9119880" y="33384960"/>
-          <a:ext cx="1069200" cy="1675800"/>
+          <a:off x="9119160" y="33384960"/>
+          <a:ext cx="1068840" cy="1675440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2472,16 +2486,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>-720</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>210600</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>95400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>187920</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2490,8 +2504,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8695080" y="2381400"/>
-          <a:ext cx="1249920" cy="1009080"/>
+          <a:off x="8694360" y="2381400"/>
+          <a:ext cx="1249560" cy="1008720"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2542,9 +2556,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>210600</xdr:colOff>
+      <xdr:colOff>210240</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2554,7 +2568,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10902240" y="2552760"/>
-          <a:ext cx="336960" cy="837720"/>
+          <a:ext cx="336600" cy="837360"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2599,15 +2613,15 @@
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>84</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
+      <xdr:colOff>75600</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>28440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>87</xdr:col>
-      <xdr:colOff>132840</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2616,8 +2630,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="17892000" y="3076560"/>
-          <a:ext cx="692640" cy="294480"/>
+          <a:off x="17891280" y="3076560"/>
+          <a:ext cx="692280" cy="294120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2667,9 +2681,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>99</xdr:col>
-      <xdr:colOff>189720</xdr:colOff>
+      <xdr:colOff>189360</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2683,7 +2697,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="18787680" y="1772280"/>
-          <a:ext cx="2399040" cy="1627560"/>
+          <a:ext cx="2398680" cy="1627200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2705,7 +2719,7 @@
   </sheetPr>
   <dimension ref="F6:EG128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3487,7 +3501,7 @@
   </sheetPr>
   <dimension ref="D3:BO196"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -10269,7 +10283,7 @@
   </sheetPr>
   <dimension ref="G4:CH109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="BO1" activeCellId="0" sqref="BO1"/>
     </sheetView>
   </sheetViews>
@@ -12925,8 +12939,8 @@
   </sheetPr>
   <dimension ref="B2:GA50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BY48" activeCellId="0" sqref="BY48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BI1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BV7" activeCellId="0" sqref="BV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.01171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12963,10 +12977,10 @@
         <v>11</v>
       </c>
       <c r="EM3" s="24"/>
-      <c r="ES3" s="11" t="s">
+      <c r="ES3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="EU3" s="11" t="s">
+      <c r="EU3" s="76" t="s">
         <v>2</v>
       </c>
     </row>
@@ -12977,37 +12991,37 @@
       <c r="K4" s="4"/>
       <c r="N4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="EM4" s="11" t="s">
+      <c r="EM4" s="75" t="s">
         <v>11</v>
       </c>
       <c r="ES4" s="24"/>
       <c r="EU4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="EA5" s="75" t="s">
+      <c r="EA5" s="77" t="s">
         <v>171</v>
       </c>
-      <c r="EB5" s="75"/>
-      <c r="EC5" s="75"/>
-      <c r="ED5" s="75"/>
-      <c r="EE5" s="75"/>
-      <c r="EF5" s="75"/>
-      <c r="EG5" s="76"/>
-      <c r="EH5" s="77"/>
-      <c r="EI5" s="77"/>
-      <c r="EJ5" s="77"/>
-      <c r="EK5" s="77"/>
-      <c r="EL5" s="77"/>
-      <c r="EM5" s="78"/>
-      <c r="EN5" s="77"/>
-      <c r="EO5" s="77"/>
-      <c r="EP5" s="77"/>
-      <c r="EQ5" s="77"/>
-      <c r="ER5" s="77"/>
-      <c r="ES5" s="78"/>
-      <c r="ET5" s="79"/>
+      <c r="EB5" s="77"/>
+      <c r="EC5" s="77"/>
+      <c r="ED5" s="77"/>
+      <c r="EE5" s="77"/>
+      <c r="EF5" s="77"/>
+      <c r="EG5" s="78"/>
+      <c r="EH5" s="79"/>
+      <c r="EI5" s="79"/>
+      <c r="EJ5" s="79"/>
+      <c r="EK5" s="79"/>
+      <c r="EL5" s="79"/>
+      <c r="EM5" s="80"/>
+      <c r="EN5" s="79"/>
+      <c r="EO5" s="79"/>
+      <c r="EP5" s="79"/>
+      <c r="EQ5" s="79"/>
+      <c r="ER5" s="79"/>
+      <c r="ES5" s="80"/>
+      <c r="ET5" s="81"/>
       <c r="EU5" s="16"/>
-      <c r="EV5" s="80"/>
+      <c r="EV5" s="82"/>
       <c r="FI5" s="15"/>
       <c r="FJ5" s="15"/>
       <c r="FK5" s="15"/>
@@ -13026,10 +13040,10 @@
       <c r="FX5" s="15"/>
       <c r="FY5" s="15"/>
       <c r="FZ5" s="15"/>
-      <c r="GA5" s="81"/>
+      <c r="GA5" s="83"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="EG6" s="82"/>
+      <c r="EG6" s="84"/>
       <c r="EH6" s="26"/>
       <c r="EI6" s="26"/>
       <c r="EJ6" s="26"/>
@@ -13041,24 +13055,24 @@
       <c r="EP6" s="26"/>
       <c r="EQ6" s="26"/>
       <c r="ER6" s="26"/>
-      <c r="ES6" s="83"/>
-      <c r="EW6" s="84"/>
-      <c r="FH6" s="85"/>
-      <c r="GA6" s="81"/>
+      <c r="ES6" s="85"/>
+      <c r="EW6" s="86"/>
+      <c r="FH6" s="87"/>
+      <c r="GA6" s="83"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="EO7" s="86"/>
-      <c r="EP7" s="86"/>
-      <c r="EQ7" s="86"/>
-      <c r="ER7" s="86"/>
-      <c r="ES7" s="87"/>
-      <c r="EX7" s="84"/>
-      <c r="FG7" s="85"/>
+      <c r="EO7" s="88"/>
+      <c r="EP7" s="88"/>
+      <c r="EQ7" s="88"/>
+      <c r="ER7" s="88"/>
+      <c r="ES7" s="89"/>
+      <c r="EX7" s="86"/>
+      <c r="FG7" s="87"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="EN8" s="87"/>
-      <c r="EY8" s="84"/>
-      <c r="FF8" s="85"/>
+      <c r="EN8" s="89"/>
+      <c r="EY8" s="86"/>
+      <c r="FF8" s="87"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="W9" s="15"/>
@@ -13079,7 +13093,7 @@
       <c r="AL9" s="15"/>
       <c r="AM9" s="15"/>
       <c r="AN9" s="15"/>
-      <c r="AO9" s="88" t="n">
+      <c r="AO9" s="90" t="n">
         <v>0</v>
       </c>
       <c r="AP9" s="45" t="n">
@@ -13091,22 +13105,22 @@
       <c r="AT9" s="15"/>
       <c r="AU9" s="15"/>
       <c r="AV9" s="15"/>
-      <c r="EM9" s="87"/>
-      <c r="ES9" s="80"/>
-      <c r="ET9" s="80"/>
-      <c r="EU9" s="80"/>
-      <c r="EV9" s="80"/>
-      <c r="EW9" s="80"/>
-      <c r="EX9" s="80"/>
-      <c r="EY9" s="80" t="s">
+      <c r="EM9" s="89"/>
+      <c r="ES9" s="82"/>
+      <c r="ET9" s="82"/>
+      <c r="EU9" s="82"/>
+      <c r="EV9" s="82"/>
+      <c r="EW9" s="82"/>
+      <c r="EX9" s="82"/>
+      <c r="EY9" s="82" t="s">
         <v>172</v>
       </c>
-      <c r="EZ9" s="89"/>
+      <c r="EZ9" s="91"/>
       <c r="FA9" s="15"/>
       <c r="FB9" s="15"/>
       <c r="FC9" s="15"/>
       <c r="FD9" s="15"/>
-      <c r="FE9" s="90"/>
+      <c r="FE9" s="92"/>
       <c r="FF9" s="15" t="s">
         <v>173</v>
       </c>
@@ -13130,113 +13144,113 @@
       <c r="FX9" s="15"/>
       <c r="FY9" s="15"/>
       <c r="FZ9" s="15"/>
-      <c r="GA9" s="81"/>
+      <c r="GA9" s="83"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="V10" s="85"/>
-      <c r="AW10" s="84"/>
-      <c r="EL10" s="91"/>
-      <c r="ER10" s="85"/>
-      <c r="GA10" s="81"/>
+      <c r="V10" s="87"/>
+      <c r="AW10" s="86"/>
+      <c r="EL10" s="93"/>
+      <c r="ER10" s="87"/>
+      <c r="GA10" s="83"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="R11" s="11" t="s">
+      <c r="R11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="U11" s="85"/>
-      <c r="AX11" s="84"/>
-      <c r="BB11" s="11" t="s">
+      <c r="U11" s="87"/>
+      <c r="AX11" s="86"/>
+      <c r="BB11" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="BI11" s="11" t="s">
+      <c r="BI11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="BP11" s="11" t="s">
+      <c r="BP11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="BX11" s="11" t="s">
+      <c r="BX11" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="BZ11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="BZ11" s="11" t="s">
+      <c r="CH11" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="CH11" s="11" t="s">
+      <c r="CT11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="CT11" s="11" t="s">
+      <c r="DK11" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="DK11" s="11" t="s">
+      <c r="DW11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="DW11" s="11" t="s">
+      <c r="EG11" s="24"/>
+      <c r="EL11" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="EG11" s="24"/>
-      <c r="EL11" s="11" t="s">
+      <c r="EN11" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="EN11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="EQ11" s="85"/>
+      <c r="EQ11" s="87"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M12" s="24"/>
       <c r="R12" s="4"/>
-      <c r="T12" s="85"/>
-      <c r="AY12" s="84"/>
-      <c r="BB12" s="11" t="s">
+      <c r="T12" s="87"/>
+      <c r="AY12" s="86"/>
+      <c r="BB12" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="BE12" s="92" t="n">
+      <c r="BE12" s="94" t="n">
         <v>8</v>
       </c>
       <c r="BF12" s="34" t="n">
         <v>9</v>
       </c>
       <c r="BI12" s="4"/>
-      <c r="BP12" s="11" t="s">
+      <c r="BP12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BS12" s="92" t="n">
+      <c r="BS12" s="94" t="n">
         <v>10</v>
       </c>
-      <c r="BX12" s="11" t="s">
+      <c r="BX12" s="75" t="s">
+        <v>175</v>
+      </c>
+      <c r="BZ12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BZ12" s="11" t="s">
+      <c r="CE12" s="94" t="n">
         <v>11</v>
       </c>
-      <c r="CE12" s="92" t="n">
+      <c r="CH12" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="CH12" s="11" t="s">
+      <c r="CT12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="CT12" s="11" t="s">
+      <c r="DK12" s="24"/>
+      <c r="DN12" s="94" t="n">
+        <v>12</v>
+      </c>
+      <c r="DW12" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="DK12" s="24"/>
-      <c r="DN12" s="92" t="n">
-        <v>12</v>
-      </c>
-      <c r="DW12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="EE12" s="92" t="n">
+      <c r="EE12" s="94" t="n">
         <v>13</v>
       </c>
-      <c r="EG12" s="11" t="s">
+      <c r="EG12" s="75" t="s">
         <v>11</v>
       </c>
       <c r="EL12" s="24"/>
       <c r="EN12" s="4"/>
-      <c r="EP12" s="85"/>
-      <c r="ER12" s="92" t="n">
+      <c r="EP12" s="87"/>
+      <c r="ER12" s="94" t="n">
         <v>4</v>
       </c>
       <c r="ES12" s="34" t="n">
@@ -13244,25 +13258,25 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E13" s="75" t="s">
-        <v>174</v>
-      </c>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
-      <c r="H13" s="75"/>
-      <c r="I13" s="75"/>
-      <c r="J13" s="90"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="78"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="79"/>
-      <c r="P13" s="79"/>
-      <c r="Q13" s="79"/>
+      <c r="E13" s="77" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="77"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="81"/>
       <c r="R13" s="16"/>
-      <c r="S13" s="90"/>
+      <c r="S13" s="92"/>
       <c r="T13" s="15" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
@@ -13297,106 +13311,106 @@
       <c r="AY13" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="AZ13" s="93"/>
+      <c r="AZ13" s="95"/>
       <c r="BA13" s="15"/>
-      <c r="BB13" s="94"/>
+      <c r="BB13" s="96"/>
       <c r="BC13" s="15"/>
       <c r="BD13" s="15" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="BE13" s="15"/>
       <c r="BF13" s="15"/>
       <c r="BG13" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="BH13" s="15"/>
+      <c r="BI13" s="97"/>
+      <c r="BJ13" s="81"/>
+      <c r="BK13" s="81"/>
+      <c r="BL13" s="81"/>
+      <c r="BM13" s="81"/>
+      <c r="BN13" s="81"/>
+      <c r="BO13" s="81"/>
+      <c r="BP13" s="98"/>
+      <c r="BQ13" s="99"/>
+      <c r="BR13" s="99"/>
+      <c r="BS13" s="99"/>
+      <c r="BT13" s="99"/>
+      <c r="BU13" s="99"/>
+      <c r="BV13" s="99"/>
+      <c r="BW13" s="99"/>
+      <c r="BX13" s="100"/>
+      <c r="BY13" s="99"/>
+      <c r="BZ13" s="97"/>
+      <c r="CA13" s="81"/>
+      <c r="CB13" s="81"/>
+      <c r="CC13" s="81"/>
+      <c r="CD13" s="81"/>
+      <c r="CE13" s="81"/>
+      <c r="CF13" s="81"/>
+      <c r="CG13" s="81"/>
+      <c r="CH13" s="80"/>
+      <c r="CI13" s="81"/>
+      <c r="CJ13" s="81"/>
+      <c r="CK13" s="81"/>
+      <c r="CL13" s="81"/>
+      <c r="CM13" s="81"/>
+      <c r="CN13" s="81"/>
+      <c r="CO13" s="81"/>
+      <c r="CP13" s="81"/>
+      <c r="CQ13" s="81"/>
+      <c r="CR13" s="81"/>
+      <c r="CS13" s="81"/>
+      <c r="CT13" s="101"/>
+      <c r="CU13" s="99"/>
+      <c r="CV13" s="99"/>
+      <c r="CW13" s="99"/>
+      <c r="CX13" s="99"/>
+      <c r="CY13" s="99"/>
+      <c r="CZ13" s="99"/>
+      <c r="DA13" s="99"/>
+      <c r="DB13" s="99"/>
+      <c r="DC13" s="99"/>
+      <c r="DD13" s="99"/>
+      <c r="DE13" s="99"/>
+      <c r="DF13" s="99"/>
+      <c r="DG13" s="99"/>
+      <c r="DH13" s="99"/>
+      <c r="DI13" s="99"/>
+      <c r="DJ13" s="99"/>
+      <c r="DK13" s="100"/>
+      <c r="DL13" s="99"/>
+      <c r="DM13" s="99"/>
+      <c r="DN13" s="99"/>
+      <c r="DO13" s="99"/>
+      <c r="DP13" s="99"/>
+      <c r="DQ13" s="99"/>
+      <c r="DR13" s="99"/>
+      <c r="DS13" s="99"/>
+      <c r="DT13" s="99"/>
+      <c r="DU13" s="99"/>
+      <c r="DV13" s="99"/>
+      <c r="DW13" s="102"/>
+      <c r="DX13" s="81"/>
+      <c r="DY13" s="81"/>
+      <c r="DZ13" s="81"/>
+      <c r="EA13" s="81"/>
+      <c r="EB13" s="81"/>
+      <c r="EC13" s="81"/>
+      <c r="ED13" s="81"/>
+      <c r="EE13" s="81"/>
+      <c r="EF13" s="81"/>
+      <c r="EG13" s="80"/>
+      <c r="EH13" s="81"/>
+      <c r="EI13" s="81"/>
+      <c r="EJ13" s="81"/>
+      <c r="EK13" s="81"/>
+      <c r="EL13" s="80"/>
+      <c r="EM13" s="81"/>
+      <c r="EN13" s="16"/>
+      <c r="EO13" s="92"/>
+      <c r="EP13" s="15" t="s">
         <v>177</v>
-      </c>
-      <c r="BH13" s="15"/>
-      <c r="BI13" s="95"/>
-      <c r="BJ13" s="79"/>
-      <c r="BK13" s="79"/>
-      <c r="BL13" s="79"/>
-      <c r="BM13" s="79"/>
-      <c r="BN13" s="79"/>
-      <c r="BO13" s="79"/>
-      <c r="BP13" s="96"/>
-      <c r="BQ13" s="97"/>
-      <c r="BR13" s="97"/>
-      <c r="BS13" s="97"/>
-      <c r="BT13" s="97"/>
-      <c r="BU13" s="97"/>
-      <c r="BV13" s="97"/>
-      <c r="BW13" s="97"/>
-      <c r="BX13" s="98"/>
-      <c r="BY13" s="97"/>
-      <c r="BZ13" s="95"/>
-      <c r="CA13" s="79"/>
-      <c r="CB13" s="79"/>
-      <c r="CC13" s="79"/>
-      <c r="CD13" s="79"/>
-      <c r="CE13" s="79"/>
-      <c r="CF13" s="79"/>
-      <c r="CG13" s="79"/>
-      <c r="CH13" s="78"/>
-      <c r="CI13" s="79"/>
-      <c r="CJ13" s="79"/>
-      <c r="CK13" s="79"/>
-      <c r="CL13" s="79"/>
-      <c r="CM13" s="79"/>
-      <c r="CN13" s="79"/>
-      <c r="CO13" s="79"/>
-      <c r="CP13" s="79"/>
-      <c r="CQ13" s="79"/>
-      <c r="CR13" s="79"/>
-      <c r="CS13" s="79"/>
-      <c r="CT13" s="99"/>
-      <c r="CU13" s="97"/>
-      <c r="CV13" s="97"/>
-      <c r="CW13" s="97"/>
-      <c r="CX13" s="97"/>
-      <c r="CY13" s="97"/>
-      <c r="CZ13" s="97"/>
-      <c r="DA13" s="97"/>
-      <c r="DB13" s="97"/>
-      <c r="DC13" s="97"/>
-      <c r="DD13" s="97"/>
-      <c r="DE13" s="97"/>
-      <c r="DF13" s="97"/>
-      <c r="DG13" s="97"/>
-      <c r="DH13" s="97"/>
-      <c r="DI13" s="97"/>
-      <c r="DJ13" s="97"/>
-      <c r="DK13" s="98"/>
-      <c r="DL13" s="97"/>
-      <c r="DM13" s="97"/>
-      <c r="DN13" s="97"/>
-      <c r="DO13" s="97"/>
-      <c r="DP13" s="97"/>
-      <c r="DQ13" s="97"/>
-      <c r="DR13" s="97"/>
-      <c r="DS13" s="97"/>
-      <c r="DT13" s="97"/>
-      <c r="DU13" s="97"/>
-      <c r="DV13" s="97"/>
-      <c r="DW13" s="100"/>
-      <c r="DX13" s="79"/>
-      <c r="DY13" s="79"/>
-      <c r="DZ13" s="79"/>
-      <c r="EA13" s="79"/>
-      <c r="EB13" s="79"/>
-      <c r="EC13" s="79"/>
-      <c r="ED13" s="79"/>
-      <c r="EE13" s="79"/>
-      <c r="EF13" s="79"/>
-      <c r="EG13" s="78"/>
-      <c r="EH13" s="79"/>
-      <c r="EI13" s="79"/>
-      <c r="EJ13" s="79"/>
-      <c r="EK13" s="79"/>
-      <c r="EL13" s="78"/>
-      <c r="EM13" s="79"/>
-      <c r="EN13" s="16"/>
-      <c r="EO13" s="90"/>
-      <c r="EP13" s="15" t="s">
-        <v>175</v>
       </c>
       <c r="EQ13" s="15"/>
       <c r="ER13" s="15"/>
@@ -13434,23 +13448,23 @@
       <c r="FX13" s="15"/>
       <c r="FY13" s="15"/>
       <c r="FZ13" s="15"/>
-      <c r="GA13" s="81"/>
+      <c r="GA13" s="83"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J14" s="84"/>
+      <c r="J14" s="86"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="102"/>
+      <c r="N14" s="103"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="104"/>
       <c r="BC14" s="34"/>
       <c r="BD14" s="43"/>
       <c r="BE14" s="34"/>
       <c r="BF14" s="34"/>
       <c r="BG14" s="33"/>
       <c r="BH14" s="34"/>
-      <c r="BI14" s="103"/>
+      <c r="BI14" s="105"/>
       <c r="BJ14" s="34"/>
       <c r="BK14" s="34"/>
       <c r="BL14" s="34"/>
@@ -13475,7 +13489,7 @@
       <c r="CE14" s="26"/>
       <c r="CF14" s="26"/>
       <c r="CG14" s="26"/>
-      <c r="CH14" s="104"/>
+      <c r="CH14" s="106"/>
       <c r="CI14" s="34"/>
       <c r="CJ14" s="34"/>
       <c r="CK14" s="34"/>
@@ -13483,8 +13497,8 @@
       <c r="CM14" s="34"/>
       <c r="CN14" s="34"/>
       <c r="CO14" s="43"/>
-      <c r="CP14" s="102" t="s">
-        <v>178</v>
+      <c r="CP14" s="104" t="s">
+        <v>180</v>
       </c>
       <c r="CQ14" s="34"/>
       <c r="CR14" s="34"/>
@@ -13510,16 +13524,16 @@
       <c r="DL14" s="26"/>
       <c r="DM14" s="26"/>
       <c r="DN14" s="26"/>
-      <c r="DO14" s="105" t="s">
-        <v>179</v>
-      </c>
-      <c r="DP14" s="106"/>
+      <c r="DO14" s="107" t="s">
+        <v>181</v>
+      </c>
+      <c r="DP14" s="108"/>
       <c r="DQ14" s="26"/>
       <c r="DR14" s="26"/>
       <c r="DS14" s="26"/>
       <c r="DT14" s="26"/>
       <c r="DU14" s="26"/>
-      <c r="DV14" s="104"/>
+      <c r="DV14" s="106"/>
       <c r="DW14" s="26"/>
       <c r="DX14" s="26"/>
       <c r="DY14" s="26"/>
@@ -13535,93 +13549,93 @@
       <c r="EI14" s="26"/>
       <c r="EJ14" s="26"/>
       <c r="EK14" s="26"/>
-      <c r="EL14" s="104"/>
-      <c r="ES14" s="84"/>
+      <c r="EL14" s="106"/>
+      <c r="ES14" s="86"/>
       <c r="ET14" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="GA14" s="81"/>
+        <v>182</v>
+      </c>
+      <c r="GA14" s="83"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N15" s="107"/>
-      <c r="P15" s="84"/>
-      <c r="Q15" s="102"/>
-      <c r="S15" s="11" t="s">
+      <c r="N15" s="109"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="104"/>
+      <c r="S15" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="BB15" s="11" t="s">
+      <c r="BB15" s="75" t="s">
         <v>2</v>
       </c>
       <c r="BE15" s="43"/>
       <c r="BF15" s="33"/>
-      <c r="BI15" s="11" t="s">
+      <c r="BI15" s="76" t="s">
         <v>2</v>
       </c>
       <c r="BN15" s="4"/>
       <c r="CD15" s="34" t="n">
         <v>14</v>
       </c>
-      <c r="CH15" s="91"/>
+      <c r="CH15" s="93"/>
       <c r="CL15" s="34" t="n">
         <v>15</v>
       </c>
       <c r="CO15" s="34"/>
-      <c r="CP15" s="84"/>
-      <c r="CQ15" s="102"/>
-      <c r="CT15" s="11" t="s">
+      <c r="CP15" s="86"/>
+      <c r="CQ15" s="104"/>
+      <c r="CT15" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="DK15" s="11" t="s">
+      <c r="DK15" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="DN15" s="108"/>
-      <c r="DO15" s="85"/>
+      <c r="DN15" s="110"/>
+      <c r="DO15" s="87"/>
       <c r="DP15" s="26"/>
       <c r="DS15" s="34" t="n">
         <v>16</v>
       </c>
-      <c r="DV15" s="91"/>
-      <c r="EL15" s="91"/>
-      <c r="ET15" s="84"/>
+      <c r="DV15" s="93"/>
+      <c r="EL15" s="93"/>
+      <c r="ET15" s="86"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N16" s="107"/>
-      <c r="Q16" s="84"/>
-      <c r="R16" s="102"/>
+      <c r="N16" s="109"/>
+      <c r="Q16" s="86"/>
+      <c r="R16" s="104"/>
       <c r="S16" s="4"/>
-      <c r="BB16" s="11" t="s">
+      <c r="BB16" s="75" t="s">
         <v>11</v>
       </c>
       <c r="BE16" s="33"/>
       <c r="BF16" s="43"/>
       <c r="BI16" s="4"/>
-      <c r="BN16" s="11" t="s">
+      <c r="BN16" s="76" t="s">
         <v>11</v>
       </c>
-      <c r="BR16" s="92" t="n">
+      <c r="BR16" s="94" t="n">
         <v>6</v>
       </c>
       <c r="BS16" s="34" t="n">
         <v>7</v>
       </c>
-      <c r="CH16" s="91"/>
+      <c r="CH16" s="93"/>
       <c r="CP16" s="34"/>
-      <c r="CQ16" s="84"/>
-      <c r="CR16" s="102"/>
-      <c r="CT16" s="11" t="s">
+      <c r="CQ16" s="86"/>
+      <c r="CR16" s="104"/>
+      <c r="CT16" s="76" t="s">
         <v>11</v>
       </c>
       <c r="DK16" s="24"/>
-      <c r="DM16" s="108"/>
-      <c r="DN16" s="85"/>
+      <c r="DM16" s="110"/>
+      <c r="DN16" s="87"/>
       <c r="DO16" s="26"/>
-      <c r="DV16" s="91"/>
-      <c r="EL16" s="91"/>
-      <c r="EU16" s="84"/>
+      <c r="DV16" s="93"/>
+      <c r="EL16" s="93"/>
+      <c r="EU16" s="86"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N17" s="107"/>
-      <c r="R17" s="84"/>
+      <c r="N17" s="109"/>
+      <c r="R17" s="86"/>
       <c r="S17" s="16"/>
       <c r="T17" s="15"/>
       <c r="U17" s="15"/>
@@ -13644,7 +13658,7 @@
       <c r="AL17" s="15"/>
       <c r="AM17" s="15"/>
       <c r="AN17" s="15"/>
-      <c r="AO17" s="88" t="n">
+      <c r="AO17" s="90" t="n">
         <v>2</v>
       </c>
       <c r="AP17" s="45" t="n">
@@ -13661,84 +13675,84 @@
       <c r="AY17" s="15"/>
       <c r="AZ17" s="15"/>
       <c r="BA17" s="15"/>
-      <c r="BB17" s="94"/>
+      <c r="BB17" s="96"/>
       <c r="BC17" s="15"/>
       <c r="BD17" s="44"/>
       <c r="BE17" s="15"/>
       <c r="BF17" s="15"/>
-      <c r="BG17" s="109"/>
+      <c r="BG17" s="111"/>
       <c r="BH17" s="15"/>
-      <c r="BI17" s="95"/>
-      <c r="BJ17" s="79"/>
-      <c r="BK17" s="79"/>
-      <c r="BL17" s="79"/>
-      <c r="BM17" s="79"/>
-      <c r="BN17" s="95"/>
-      <c r="BO17" s="79"/>
-      <c r="BP17" s="79"/>
-      <c r="BQ17" s="93"/>
-      <c r="BR17" s="75" t="s">
-        <v>181</v>
-      </c>
-      <c r="BS17" s="75"/>
-      <c r="BT17" s="75"/>
-      <c r="BU17" s="75"/>
-      <c r="BV17" s="75"/>
-      <c r="BW17" s="75"/>
-      <c r="CH17" s="91"/>
-      <c r="CL17" s="110"/>
+      <c r="BI17" s="97"/>
+      <c r="BJ17" s="81"/>
+      <c r="BK17" s="81"/>
+      <c r="BL17" s="81"/>
+      <c r="BM17" s="81"/>
+      <c r="BN17" s="97"/>
+      <c r="BO17" s="81"/>
+      <c r="BP17" s="81"/>
+      <c r="BQ17" s="95"/>
+      <c r="BR17" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="BS17" s="77"/>
+      <c r="BT17" s="77"/>
+      <c r="BU17" s="77"/>
+      <c r="BV17" s="77"/>
+      <c r="BW17" s="77"/>
+      <c r="CH17" s="93"/>
+      <c r="CL17" s="112"/>
       <c r="CM17" s="15"/>
       <c r="CN17" s="15"/>
       <c r="CO17" s="15"/>
       <c r="CP17" s="15"/>
-      <c r="CQ17" s="111" t="s">
-        <v>182</v>
-      </c>
-      <c r="CR17" s="93"/>
-      <c r="CS17" s="79"/>
-      <c r="CT17" s="99"/>
-      <c r="CU17" s="97"/>
-      <c r="CV17" s="97"/>
-      <c r="CW17" s="97"/>
-      <c r="CX17" s="97"/>
-      <c r="CY17" s="97"/>
-      <c r="CZ17" s="97"/>
-      <c r="DA17" s="97"/>
-      <c r="DB17" s="97"/>
-      <c r="DC17" s="97"/>
-      <c r="DD17" s="97"/>
-      <c r="DE17" s="97"/>
-      <c r="DF17" s="97"/>
-      <c r="DG17" s="97"/>
-      <c r="DH17" s="97"/>
-      <c r="DI17" s="97"/>
-      <c r="DJ17" s="97"/>
-      <c r="DK17" s="98"/>
-      <c r="DL17" s="97"/>
-      <c r="DM17" s="90"/>
-      <c r="DN17" s="112" t="s">
-        <v>183</v>
+      <c r="CQ17" s="113" t="s">
+        <v>184</v>
+      </c>
+      <c r="CR17" s="95"/>
+      <c r="CS17" s="81"/>
+      <c r="CT17" s="101"/>
+      <c r="CU17" s="99"/>
+      <c r="CV17" s="99"/>
+      <c r="CW17" s="99"/>
+      <c r="CX17" s="99"/>
+      <c r="CY17" s="99"/>
+      <c r="CZ17" s="99"/>
+      <c r="DA17" s="99"/>
+      <c r="DB17" s="99"/>
+      <c r="DC17" s="99"/>
+      <c r="DD17" s="99"/>
+      <c r="DE17" s="99"/>
+      <c r="DF17" s="99"/>
+      <c r="DG17" s="99"/>
+      <c r="DH17" s="99"/>
+      <c r="DI17" s="99"/>
+      <c r="DJ17" s="99"/>
+      <c r="DK17" s="100"/>
+      <c r="DL17" s="99"/>
+      <c r="DM17" s="92"/>
+      <c r="DN17" s="114" t="s">
+        <v>185</v>
       </c>
       <c r="DO17" s="15"/>
       <c r="DP17" s="15"/>
       <c r="DQ17" s="15"/>
       <c r="DR17" s="15"/>
       <c r="DS17" s="15"/>
-      <c r="DT17" s="81"/>
-      <c r="DV17" s="91"/>
-      <c r="EL17" s="91"/>
-      <c r="EV17" s="84"/>
-      <c r="EW17" s="113"/>
-      <c r="EX17" s="113"/>
-      <c r="EY17" s="113"/>
-      <c r="EZ17" s="113"/>
-      <c r="FA17" s="113"/>
-      <c r="FB17" s="113"/>
-      <c r="FC17" s="113"/>
-      <c r="FD17" s="113"/>
-      <c r="FE17" s="113"/>
-      <c r="FF17" s="113"/>
-      <c r="FG17" s="113"/>
+      <c r="DT17" s="83"/>
+      <c r="DV17" s="93"/>
+      <c r="EL17" s="93"/>
+      <c r="EV17" s="86"/>
+      <c r="EW17" s="115"/>
+      <c r="EX17" s="115"/>
+      <c r="EY17" s="115"/>
+      <c r="EZ17" s="115"/>
+      <c r="FA17" s="115"/>
+      <c r="FB17" s="115"/>
+      <c r="FC17" s="115"/>
+      <c r="FD17" s="115"/>
+      <c r="FE17" s="115"/>
+      <c r="FF17" s="115"/>
+      <c r="FG17" s="115"/>
       <c r="FH17" s="15"/>
       <c r="FI17" s="15"/>
       <c r="FJ17" s="15"/>
@@ -13758,29 +13772,29 @@
       <c r="FX17" s="15"/>
       <c r="FY17" s="15"/>
       <c r="FZ17" s="15"/>
-      <c r="GA17" s="81"/>
+      <c r="GA17" s="83"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N18" s="107"/>
-      <c r="S18" s="84"/>
+      <c r="N18" s="109"/>
+      <c r="S18" s="86"/>
       <c r="T18" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="AY18" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="AZ18" s="85"/>
+      <c r="AZ18" s="87"/>
       <c r="BC18" s="34"/>
       <c r="BD18" s="34" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="BE18" s="34"/>
       <c r="BF18" s="34"/>
       <c r="BG18" s="34" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="BH18" s="34"/>
-      <c r="BI18" s="103"/>
+      <c r="BI18" s="105"/>
       <c r="BJ18" s="34"/>
       <c r="BK18" s="34"/>
       <c r="BL18" s="34"/>
@@ -13788,9 +13802,9 @@
       <c r="BN18" s="34"/>
       <c r="BO18" s="34"/>
       <c r="BP18" s="34"/>
-      <c r="BQ18" s="85"/>
-      <c r="CH18" s="91"/>
-      <c r="CL18" s="81"/>
+      <c r="BQ18" s="87"/>
+      <c r="CH18" s="93"/>
+      <c r="CL18" s="83"/>
       <c r="CR18" s="34"/>
       <c r="CS18" s="34"/>
       <c r="CT18" s="34"/>
@@ -13813,32 +13827,32 @@
       <c r="DK18" s="34"/>
       <c r="DL18" s="26"/>
       <c r="DM18" s="26"/>
-      <c r="DT18" s="81"/>
-      <c r="DV18" s="91"/>
-      <c r="EL18" s="91"/>
-      <c r="GA18" s="81"/>
+      <c r="DT18" s="83"/>
+      <c r="DV18" s="93"/>
+      <c r="EL18" s="93"/>
+      <c r="GA18" s="83"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N19" s="107"/>
-      <c r="T19" s="84"/>
-      <c r="AY19" s="85"/>
-      <c r="BI19" s="107"/>
-      <c r="CH19" s="91"/>
-      <c r="DV19" s="91"/>
-      <c r="EL19" s="91"/>
+      <c r="N19" s="109"/>
+      <c r="T19" s="86"/>
+      <c r="AY19" s="87"/>
+      <c r="BI19" s="109"/>
+      <c r="CH19" s="93"/>
+      <c r="DV19" s="93"/>
+      <c r="EL19" s="93"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N20" s="107"/>
-      <c r="U20" s="84"/>
-      <c r="AX20" s="85"/>
-      <c r="BI20" s="107"/>
-      <c r="CH20" s="91"/>
-      <c r="DV20" s="91"/>
-      <c r="EL20" s="91"/>
+      <c r="N20" s="109"/>
+      <c r="U20" s="86"/>
+      <c r="AX20" s="87"/>
+      <c r="BI20" s="109"/>
+      <c r="CH20" s="93"/>
+      <c r="DV20" s="93"/>
+      <c r="EL20" s="93"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N21" s="107"/>
-      <c r="V21" s="84"/>
+      <c r="N21" s="109"/>
+      <c r="V21" s="86"/>
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
@@ -13865,333 +13879,333 @@
       <c r="AT21" s="15"/>
       <c r="AU21" s="15"/>
       <c r="AV21" s="15"/>
-      <c r="AW21" s="85"/>
-      <c r="BI21" s="107"/>
-      <c r="CH21" s="91"/>
-      <c r="DV21" s="91"/>
-      <c r="EL21" s="91"/>
+      <c r="AW21" s="87"/>
+      <c r="BI21" s="109"/>
+      <c r="CH21" s="93"/>
+      <c r="DV21" s="93"/>
+      <c r="EL21" s="93"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N22" s="107"/>
-      <c r="BI22" s="107"/>
-      <c r="CH22" s="91"/>
-      <c r="DV22" s="91"/>
-      <c r="EL22" s="91"/>
+      <c r="N22" s="109"/>
+      <c r="BI22" s="109"/>
+      <c r="CH22" s="93"/>
+      <c r="DV22" s="93"/>
+      <c r="EL22" s="93"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N23" s="107"/>
-      <c r="BI23" s="107"/>
+      <c r="N23" s="109"/>
+      <c r="BI23" s="109"/>
       <c r="BS23" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="CH23" s="91"/>
-      <c r="DV23" s="91"/>
-      <c r="EL23" s="91"/>
+        <v>188</v>
+      </c>
+      <c r="CH23" s="93"/>
+      <c r="DV23" s="93"/>
+      <c r="EL23" s="93"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N24" s="107"/>
-      <c r="BI24" s="107"/>
-      <c r="CH24" s="91"/>
-      <c r="DV24" s="91"/>
-      <c r="EL24" s="91"/>
+      <c r="N24" s="109"/>
+      <c r="BI24" s="109"/>
+      <c r="CH24" s="93"/>
+      <c r="DV24" s="93"/>
+      <c r="EL24" s="93"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N25" s="107"/>
-      <c r="BI25" s="107"/>
-      <c r="CH25" s="91"/>
-      <c r="DV25" s="91"/>
-      <c r="EL25" s="91"/>
+      <c r="N25" s="109"/>
+      <c r="BI25" s="109"/>
+      <c r="CH25" s="93"/>
+      <c r="DV25" s="93"/>
+      <c r="EL25" s="93"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N26" s="107"/>
-      <c r="BI26" s="107"/>
-      <c r="CH26" s="91"/>
-      <c r="DV26" s="91"/>
-      <c r="EL26" s="91"/>
+      <c r="N26" s="109"/>
+      <c r="BI26" s="109"/>
+      <c r="CH26" s="93"/>
+      <c r="DV26" s="93"/>
+      <c r="EL26" s="93"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N27" s="107"/>
-      <c r="BI27" s="107"/>
-      <c r="CH27" s="91"/>
-      <c r="DV27" s="91"/>
-      <c r="EL27" s="91"/>
+      <c r="N27" s="109"/>
+      <c r="BI27" s="109"/>
+      <c r="CH27" s="93"/>
+      <c r="DV27" s="93"/>
+      <c r="EL27" s="93"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N28" s="107"/>
-      <c r="BI28" s="107"/>
-      <c r="CH28" s="91"/>
-      <c r="DV28" s="91"/>
-      <c r="EL28" s="91"/>
+      <c r="N28" s="109"/>
+      <c r="BI28" s="109"/>
+      <c r="CH28" s="93"/>
+      <c r="DV28" s="93"/>
+      <c r="EL28" s="93"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N29" s="114" t="s">
-        <v>187</v>
-      </c>
-      <c r="O29" s="114"/>
-      <c r="P29" s="114"/>
-      <c r="Q29" s="114"/>
-      <c r="R29" s="114"/>
-      <c r="S29" s="114"/>
-      <c r="T29" s="114"/>
-      <c r="U29" s="114"/>
-      <c r="V29" s="114"/>
-      <c r="W29" s="114"/>
-      <c r="X29" s="114"/>
-      <c r="Y29" s="114"/>
-      <c r="Z29" s="114"/>
-      <c r="AA29" s="114"/>
-      <c r="AB29" s="114"/>
-      <c r="AC29" s="114"/>
-      <c r="AD29" s="114"/>
-      <c r="AE29" s="114"/>
-      <c r="AF29" s="114"/>
-      <c r="AG29" s="114"/>
-      <c r="AH29" s="114"/>
-      <c r="AI29" s="114"/>
-      <c r="AJ29" s="114"/>
-      <c r="AK29" s="114"/>
-      <c r="AL29" s="114"/>
-      <c r="AM29" s="114"/>
-      <c r="AN29" s="114"/>
-      <c r="AO29" s="114"/>
-      <c r="AP29" s="114"/>
-      <c r="AQ29" s="114"/>
-      <c r="AR29" s="114"/>
-      <c r="AS29" s="114"/>
-      <c r="AT29" s="114"/>
-      <c r="AU29" s="114"/>
-      <c r="AV29" s="114"/>
-      <c r="AW29" s="114"/>
-      <c r="AX29" s="114"/>
-      <c r="AY29" s="114"/>
-      <c r="AZ29" s="114"/>
-      <c r="BA29" s="114"/>
-      <c r="BB29" s="114"/>
-      <c r="BC29" s="114"/>
-      <c r="BD29" s="114"/>
-      <c r="BE29" s="114"/>
-      <c r="BF29" s="114"/>
-      <c r="BG29" s="114"/>
-      <c r="BH29" s="114"/>
-      <c r="BI29" s="107"/>
-      <c r="CH29" s="91"/>
-      <c r="CI29" s="114" t="s">
-        <v>188</v>
-      </c>
-      <c r="CJ29" s="114"/>
-      <c r="CK29" s="114"/>
-      <c r="CL29" s="114"/>
-      <c r="CM29" s="114"/>
-      <c r="CN29" s="114"/>
-      <c r="CO29" s="114"/>
-      <c r="CP29" s="114"/>
-      <c r="CQ29" s="114"/>
-      <c r="CR29" s="114"/>
-      <c r="CS29" s="114"/>
-      <c r="CT29" s="114"/>
-      <c r="CU29" s="114"/>
-      <c r="CV29" s="114"/>
-      <c r="CW29" s="114"/>
-      <c r="CX29" s="114"/>
-      <c r="CY29" s="114"/>
-      <c r="CZ29" s="114"/>
-      <c r="DA29" s="114"/>
-      <c r="DB29" s="114"/>
-      <c r="DC29" s="114"/>
-      <c r="DD29" s="114"/>
-      <c r="DE29" s="114"/>
-      <c r="DF29" s="114"/>
-      <c r="DG29" s="114"/>
-      <c r="DH29" s="114"/>
-      <c r="DI29" s="114"/>
-      <c r="DJ29" s="114"/>
-      <c r="DK29" s="114"/>
-      <c r="DL29" s="114"/>
-      <c r="DM29" s="114"/>
-      <c r="DN29" s="114"/>
-      <c r="DO29" s="114"/>
-      <c r="DP29" s="114"/>
-      <c r="DQ29" s="114"/>
-      <c r="DR29" s="114"/>
-      <c r="DS29" s="114"/>
-      <c r="DT29" s="114"/>
-      <c r="DU29" s="114"/>
-      <c r="DV29" s="114"/>
-      <c r="EL29" s="91"/>
-      <c r="EM29" s="115" t="s">
+      <c r="N29" s="116" t="s">
         <v>189</v>
       </c>
-      <c r="EN29" s="115"/>
-      <c r="EO29" s="115"/>
-      <c r="EP29" s="115"/>
-      <c r="EQ29" s="115"/>
-      <c r="ER29" s="115"/>
-      <c r="ES29" s="115"/>
-      <c r="ET29" s="115"/>
-      <c r="EU29" s="115"/>
-      <c r="EV29" s="115"/>
-      <c r="EW29" s="115"/>
-      <c r="EX29" s="115"/>
-      <c r="EY29" s="115"/>
-      <c r="EZ29" s="115"/>
-      <c r="FA29" s="115"/>
-      <c r="FB29" s="115"/>
-      <c r="FC29" s="115"/>
-      <c r="FD29" s="115"/>
-      <c r="FE29" s="115"/>
-      <c r="FF29" s="115"/>
-      <c r="FG29" s="115"/>
-      <c r="FH29" s="115"/>
-      <c r="FI29" s="115"/>
-      <c r="FJ29" s="115"/>
-      <c r="FK29" s="115"/>
-      <c r="FL29" s="115"/>
-      <c r="FM29" s="115"/>
-      <c r="FN29" s="115"/>
-      <c r="FO29" s="115"/>
-      <c r="FP29" s="115"/>
-      <c r="FQ29" s="115"/>
-      <c r="FR29" s="115"/>
-      <c r="FS29" s="115"/>
-      <c r="FT29" s="115"/>
-      <c r="FU29" s="115"/>
-      <c r="FV29" s="115"/>
-      <c r="FW29" s="115"/>
-      <c r="FX29" s="115"/>
-      <c r="FY29" s="115"/>
-      <c r="FZ29" s="115"/>
+      <c r="O29" s="116"/>
+      <c r="P29" s="116"/>
+      <c r="Q29" s="116"/>
+      <c r="R29" s="116"/>
+      <c r="S29" s="116"/>
+      <c r="T29" s="116"/>
+      <c r="U29" s="116"/>
+      <c r="V29" s="116"/>
+      <c r="W29" s="116"/>
+      <c r="X29" s="116"/>
+      <c r="Y29" s="116"/>
+      <c r="Z29" s="116"/>
+      <c r="AA29" s="116"/>
+      <c r="AB29" s="116"/>
+      <c r="AC29" s="116"/>
+      <c r="AD29" s="116"/>
+      <c r="AE29" s="116"/>
+      <c r="AF29" s="116"/>
+      <c r="AG29" s="116"/>
+      <c r="AH29" s="116"/>
+      <c r="AI29" s="116"/>
+      <c r="AJ29" s="116"/>
+      <c r="AK29" s="116"/>
+      <c r="AL29" s="116"/>
+      <c r="AM29" s="116"/>
+      <c r="AN29" s="116"/>
+      <c r="AO29" s="116"/>
+      <c r="AP29" s="116"/>
+      <c r="AQ29" s="116"/>
+      <c r="AR29" s="116"/>
+      <c r="AS29" s="116"/>
+      <c r="AT29" s="116"/>
+      <c r="AU29" s="116"/>
+      <c r="AV29" s="116"/>
+      <c r="AW29" s="116"/>
+      <c r="AX29" s="116"/>
+      <c r="AY29" s="116"/>
+      <c r="AZ29" s="116"/>
+      <c r="BA29" s="116"/>
+      <c r="BB29" s="116"/>
+      <c r="BC29" s="116"/>
+      <c r="BD29" s="116"/>
+      <c r="BE29" s="116"/>
+      <c r="BF29" s="116"/>
+      <c r="BG29" s="116"/>
+      <c r="BH29" s="116"/>
+      <c r="BI29" s="109"/>
+      <c r="CH29" s="93"/>
+      <c r="CI29" s="116" t="s">
+        <v>190</v>
+      </c>
+      <c r="CJ29" s="116"/>
+      <c r="CK29" s="116"/>
+      <c r="CL29" s="116"/>
+      <c r="CM29" s="116"/>
+      <c r="CN29" s="116"/>
+      <c r="CO29" s="116"/>
+      <c r="CP29" s="116"/>
+      <c r="CQ29" s="116"/>
+      <c r="CR29" s="116"/>
+      <c r="CS29" s="116"/>
+      <c r="CT29" s="116"/>
+      <c r="CU29" s="116"/>
+      <c r="CV29" s="116"/>
+      <c r="CW29" s="116"/>
+      <c r="CX29" s="116"/>
+      <c r="CY29" s="116"/>
+      <c r="CZ29" s="116"/>
+      <c r="DA29" s="116"/>
+      <c r="DB29" s="116"/>
+      <c r="DC29" s="116"/>
+      <c r="DD29" s="116"/>
+      <c r="DE29" s="116"/>
+      <c r="DF29" s="116"/>
+      <c r="DG29" s="116"/>
+      <c r="DH29" s="116"/>
+      <c r="DI29" s="116"/>
+      <c r="DJ29" s="116"/>
+      <c r="DK29" s="116"/>
+      <c r="DL29" s="116"/>
+      <c r="DM29" s="116"/>
+      <c r="DN29" s="116"/>
+      <c r="DO29" s="116"/>
+      <c r="DP29" s="116"/>
+      <c r="DQ29" s="116"/>
+      <c r="DR29" s="116"/>
+      <c r="DS29" s="116"/>
+      <c r="DT29" s="116"/>
+      <c r="DU29" s="116"/>
+      <c r="DV29" s="116"/>
+      <c r="EL29" s="93"/>
+      <c r="EM29" s="117" t="s">
+        <v>191</v>
+      </c>
+      <c r="EN29" s="117"/>
+      <c r="EO29" s="117"/>
+      <c r="EP29" s="117"/>
+      <c r="EQ29" s="117"/>
+      <c r="ER29" s="117"/>
+      <c r="ES29" s="117"/>
+      <c r="ET29" s="117"/>
+      <c r="EU29" s="117"/>
+      <c r="EV29" s="117"/>
+      <c r="EW29" s="117"/>
+      <c r="EX29" s="117"/>
+      <c r="EY29" s="117"/>
+      <c r="EZ29" s="117"/>
+      <c r="FA29" s="117"/>
+      <c r="FB29" s="117"/>
+      <c r="FC29" s="117"/>
+      <c r="FD29" s="117"/>
+      <c r="FE29" s="117"/>
+      <c r="FF29" s="117"/>
+      <c r="FG29" s="117"/>
+      <c r="FH29" s="117"/>
+      <c r="FI29" s="117"/>
+      <c r="FJ29" s="117"/>
+      <c r="FK29" s="117"/>
+      <c r="FL29" s="117"/>
+      <c r="FM29" s="117"/>
+      <c r="FN29" s="117"/>
+      <c r="FO29" s="117"/>
+      <c r="FP29" s="117"/>
+      <c r="FQ29" s="117"/>
+      <c r="FR29" s="117"/>
+      <c r="FS29" s="117"/>
+      <c r="FT29" s="117"/>
+      <c r="FU29" s="117"/>
+      <c r="FV29" s="117"/>
+      <c r="FW29" s="117"/>
+      <c r="FX29" s="117"/>
+      <c r="FY29" s="117"/>
+      <c r="FZ29" s="117"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N30" s="114"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="114"/>
-      <c r="R30" s="114"/>
-      <c r="S30" s="114"/>
-      <c r="T30" s="114"/>
-      <c r="U30" s="114"/>
-      <c r="V30" s="114"/>
-      <c r="W30" s="114"/>
-      <c r="X30" s="114"/>
-      <c r="Y30" s="114"/>
-      <c r="Z30" s="114"/>
-      <c r="AA30" s="114"/>
-      <c r="AB30" s="114"/>
-      <c r="AC30" s="114"/>
-      <c r="AD30" s="114"/>
-      <c r="AE30" s="114"/>
-      <c r="AF30" s="114"/>
-      <c r="AG30" s="114"/>
-      <c r="AH30" s="114"/>
-      <c r="AI30" s="114"/>
-      <c r="AJ30" s="114"/>
-      <c r="AK30" s="114"/>
-      <c r="AL30" s="114"/>
-      <c r="AM30" s="114"/>
-      <c r="AN30" s="114"/>
-      <c r="AO30" s="114"/>
-      <c r="AP30" s="114"/>
-      <c r="AQ30" s="114"/>
-      <c r="AR30" s="114"/>
-      <c r="AS30" s="114"/>
-      <c r="AT30" s="114"/>
-      <c r="AU30" s="114"/>
-      <c r="AV30" s="114"/>
-      <c r="AW30" s="114"/>
-      <c r="AX30" s="114"/>
-      <c r="AY30" s="114"/>
-      <c r="AZ30" s="114"/>
-      <c r="BA30" s="114"/>
-      <c r="BB30" s="114"/>
-      <c r="BC30" s="114"/>
-      <c r="BD30" s="114"/>
-      <c r="BE30" s="114"/>
-      <c r="BF30" s="114"/>
-      <c r="BG30" s="114"/>
-      <c r="BH30" s="114"/>
-      <c r="BI30" s="107"/>
-      <c r="CH30" s="91"/>
-      <c r="CI30" s="114"/>
-      <c r="CJ30" s="114"/>
-      <c r="CK30" s="114"/>
-      <c r="CL30" s="114"/>
-      <c r="CM30" s="114"/>
-      <c r="CN30" s="114"/>
-      <c r="CO30" s="114"/>
-      <c r="CP30" s="114"/>
-      <c r="CQ30" s="114"/>
-      <c r="CR30" s="114"/>
-      <c r="CS30" s="114"/>
-      <c r="CT30" s="114"/>
-      <c r="CU30" s="114"/>
-      <c r="CV30" s="114"/>
-      <c r="CW30" s="114"/>
-      <c r="CX30" s="114"/>
-      <c r="CY30" s="114"/>
-      <c r="CZ30" s="114"/>
-      <c r="DA30" s="114"/>
-      <c r="DB30" s="114"/>
-      <c r="DC30" s="114"/>
-      <c r="DD30" s="114"/>
-      <c r="DE30" s="114"/>
-      <c r="DF30" s="114"/>
-      <c r="DG30" s="114"/>
-      <c r="DH30" s="114"/>
-      <c r="DI30" s="114"/>
-      <c r="DJ30" s="114"/>
-      <c r="DK30" s="114"/>
-      <c r="DL30" s="114"/>
-      <c r="DM30" s="114"/>
-      <c r="DN30" s="114"/>
-      <c r="DO30" s="114"/>
-      <c r="DP30" s="114"/>
-      <c r="DQ30" s="114"/>
-      <c r="DR30" s="114"/>
-      <c r="DS30" s="114"/>
-      <c r="DT30" s="114"/>
-      <c r="DU30" s="114"/>
-      <c r="DV30" s="114"/>
-      <c r="EL30" s="91"/>
-      <c r="EM30" s="115"/>
-      <c r="EN30" s="115"/>
-      <c r="EO30" s="115"/>
-      <c r="EP30" s="115"/>
-      <c r="EQ30" s="115"/>
-      <c r="ER30" s="115"/>
-      <c r="ES30" s="115"/>
-      <c r="ET30" s="115"/>
-      <c r="EU30" s="115"/>
-      <c r="EV30" s="115"/>
-      <c r="EW30" s="115"/>
-      <c r="EX30" s="115"/>
-      <c r="EY30" s="115"/>
-      <c r="EZ30" s="115"/>
-      <c r="FA30" s="115"/>
-      <c r="FB30" s="115"/>
-      <c r="FC30" s="115"/>
-      <c r="FD30" s="115"/>
-      <c r="FE30" s="115"/>
-      <c r="FF30" s="115"/>
-      <c r="FG30" s="115"/>
-      <c r="FH30" s="115"/>
-      <c r="FI30" s="115"/>
-      <c r="FJ30" s="115"/>
-      <c r="FK30" s="115"/>
-      <c r="FL30" s="115"/>
-      <c r="FM30" s="115"/>
-      <c r="FN30" s="115"/>
-      <c r="FO30" s="115"/>
-      <c r="FP30" s="115"/>
-      <c r="FQ30" s="115"/>
-      <c r="FR30" s="115"/>
-      <c r="FS30" s="115"/>
-      <c r="FT30" s="115"/>
-      <c r="FU30" s="115"/>
-      <c r="FV30" s="115"/>
-      <c r="FW30" s="115"/>
-      <c r="FX30" s="115"/>
-      <c r="FY30" s="115"/>
-      <c r="FZ30" s="115"/>
+      <c r="N30" s="116"/>
+      <c r="O30" s="116"/>
+      <c r="P30" s="116"/>
+      <c r="Q30" s="116"/>
+      <c r="R30" s="116"/>
+      <c r="S30" s="116"/>
+      <c r="T30" s="116"/>
+      <c r="U30" s="116"/>
+      <c r="V30" s="116"/>
+      <c r="W30" s="116"/>
+      <c r="X30" s="116"/>
+      <c r="Y30" s="116"/>
+      <c r="Z30" s="116"/>
+      <c r="AA30" s="116"/>
+      <c r="AB30" s="116"/>
+      <c r="AC30" s="116"/>
+      <c r="AD30" s="116"/>
+      <c r="AE30" s="116"/>
+      <c r="AF30" s="116"/>
+      <c r="AG30" s="116"/>
+      <c r="AH30" s="116"/>
+      <c r="AI30" s="116"/>
+      <c r="AJ30" s="116"/>
+      <c r="AK30" s="116"/>
+      <c r="AL30" s="116"/>
+      <c r="AM30" s="116"/>
+      <c r="AN30" s="116"/>
+      <c r="AO30" s="116"/>
+      <c r="AP30" s="116"/>
+      <c r="AQ30" s="116"/>
+      <c r="AR30" s="116"/>
+      <c r="AS30" s="116"/>
+      <c r="AT30" s="116"/>
+      <c r="AU30" s="116"/>
+      <c r="AV30" s="116"/>
+      <c r="AW30" s="116"/>
+      <c r="AX30" s="116"/>
+      <c r="AY30" s="116"/>
+      <c r="AZ30" s="116"/>
+      <c r="BA30" s="116"/>
+      <c r="BB30" s="116"/>
+      <c r="BC30" s="116"/>
+      <c r="BD30" s="116"/>
+      <c r="BE30" s="116"/>
+      <c r="BF30" s="116"/>
+      <c r="BG30" s="116"/>
+      <c r="BH30" s="116"/>
+      <c r="BI30" s="109"/>
+      <c r="CH30" s="93"/>
+      <c r="CI30" s="116"/>
+      <c r="CJ30" s="116"/>
+      <c r="CK30" s="116"/>
+      <c r="CL30" s="116"/>
+      <c r="CM30" s="116"/>
+      <c r="CN30" s="116"/>
+      <c r="CO30" s="116"/>
+      <c r="CP30" s="116"/>
+      <c r="CQ30" s="116"/>
+      <c r="CR30" s="116"/>
+      <c r="CS30" s="116"/>
+      <c r="CT30" s="116"/>
+      <c r="CU30" s="116"/>
+      <c r="CV30" s="116"/>
+      <c r="CW30" s="116"/>
+      <c r="CX30" s="116"/>
+      <c r="CY30" s="116"/>
+      <c r="CZ30" s="116"/>
+      <c r="DA30" s="116"/>
+      <c r="DB30" s="116"/>
+      <c r="DC30" s="116"/>
+      <c r="DD30" s="116"/>
+      <c r="DE30" s="116"/>
+      <c r="DF30" s="116"/>
+      <c r="DG30" s="116"/>
+      <c r="DH30" s="116"/>
+      <c r="DI30" s="116"/>
+      <c r="DJ30" s="116"/>
+      <c r="DK30" s="116"/>
+      <c r="DL30" s="116"/>
+      <c r="DM30" s="116"/>
+      <c r="DN30" s="116"/>
+      <c r="DO30" s="116"/>
+      <c r="DP30" s="116"/>
+      <c r="DQ30" s="116"/>
+      <c r="DR30" s="116"/>
+      <c r="DS30" s="116"/>
+      <c r="DT30" s="116"/>
+      <c r="DU30" s="116"/>
+      <c r="DV30" s="116"/>
+      <c r="EL30" s="93"/>
+      <c r="EM30" s="117"/>
+      <c r="EN30" s="117"/>
+      <c r="EO30" s="117"/>
+      <c r="EP30" s="117"/>
+      <c r="EQ30" s="117"/>
+      <c r="ER30" s="117"/>
+      <c r="ES30" s="117"/>
+      <c r="ET30" s="117"/>
+      <c r="EU30" s="117"/>
+      <c r="EV30" s="117"/>
+      <c r="EW30" s="117"/>
+      <c r="EX30" s="117"/>
+      <c r="EY30" s="117"/>
+      <c r="EZ30" s="117"/>
+      <c r="FA30" s="117"/>
+      <c r="FB30" s="117"/>
+      <c r="FC30" s="117"/>
+      <c r="FD30" s="117"/>
+      <c r="FE30" s="117"/>
+      <c r="FF30" s="117"/>
+      <c r="FG30" s="117"/>
+      <c r="FH30" s="117"/>
+      <c r="FI30" s="117"/>
+      <c r="FJ30" s="117"/>
+      <c r="FK30" s="117"/>
+      <c r="FL30" s="117"/>
+      <c r="FM30" s="117"/>
+      <c r="FN30" s="117"/>
+      <c r="FO30" s="117"/>
+      <c r="FP30" s="117"/>
+      <c r="FQ30" s="117"/>
+      <c r="FR30" s="117"/>
+      <c r="FS30" s="117"/>
+      <c r="FT30" s="117"/>
+      <c r="FU30" s="117"/>
+      <c r="FV30" s="117"/>
+      <c r="FW30" s="117"/>
+      <c r="FX30" s="117"/>
+      <c r="FY30" s="117"/>
+      <c r="FZ30" s="117"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AP36" s="0" t="n">
@@ -14229,19 +14243,19 @@
       <c r="BC37" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="BD37" s="96"/>
-      <c r="BE37" s="97"/>
-      <c r="BF37" s="97"/>
-      <c r="BG37" s="97"/>
-      <c r="BH37" s="97"/>
-      <c r="BI37" s="97"/>
-      <c r="BJ37" s="97"/>
-      <c r="BK37" s="97"/>
+      <c r="BD37" s="98"/>
+      <c r="BE37" s="99"/>
+      <c r="BF37" s="99"/>
+      <c r="BG37" s="99"/>
+      <c r="BH37" s="99"/>
+      <c r="BI37" s="99"/>
+      <c r="BJ37" s="99"/>
+      <c r="BK37" s="99"/>
       <c r="BL37" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BT37" s="2"/>
-      <c r="BU37" s="85"/>
+      <c r="BU37" s="87"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AS38" s="43"/>
@@ -14254,25 +14268,25 @@
       <c r="BI38" s="34"/>
       <c r="BJ38" s="34"/>
       <c r="BK38" s="34"/>
-      <c r="BT38" s="85"/>
+      <c r="BT38" s="87"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AS39" s="33"/>
       <c r="AT39" s="43"/>
-      <c r="BS39" s="85"/>
+      <c r="BS39" s="87"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AQ40" s="15"/>
       <c r="AR40" s="44"/>
       <c r="AS40" s="15"/>
       <c r="AT40" s="15"/>
-      <c r="AU40" s="109"/>
+      <c r="AU40" s="111"/>
       <c r="AV40" s="15"/>
       <c r="BP40" s="0" t="n">
         <v>1</v>
       </c>
       <c r="BQ40" s="15"/>
-      <c r="BR40" s="85"/>
+      <c r="BR40" s="87"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AP41" s="0" t="n">
@@ -14288,7 +14302,7 @@
         <v>3</v>
       </c>
       <c r="BS41" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -14307,23 +14321,23 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BR46" s="84"/>
+      <c r="BR46" s="86"/>
       <c r="BS46" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BS47" s="84"/>
+      <c r="BS47" s="86"/>
       <c r="BY47" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BT48" s="84"/>
+      <c r="BT48" s="86"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="BU49" s="84"/>
-      <c r="BV49" s="113"/>
+      <c r="BU49" s="86"/>
+      <c r="BV49" s="115"/>
       <c r="BW49" s="0" t="n">
         <v>2</v>
       </c>

</xml_diff>